<commit_message>
Estimated emissions from UN
</commit_message>
<xml_diff>
--- a/gears_db/data/classifications/equivalence.xlsx
+++ b/gears_db/data/classifications/equivalence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\gears\gears_db\data\classifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9A3600-5A9B-4A2E-8A99-1592BBAEEE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E3FF0E-03C6-4FD5-9DAA-0A96D94DBD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1DC89B59-BD96-4A38-B17B-1A23D20B8AC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1DC89B59-BD96-4A38-B17B-1A23D20B8AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="FAOSTAT COUNTRIES" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="1464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="1470">
   <si>
     <t>Armenia</t>
   </si>
@@ -4346,21 +4346,9 @@
     <t xml:space="preserve"> 9999</t>
   </si>
   <si>
-    <t>9.A.</t>
-  </si>
-  <si>
-    <t>3.C.7.</t>
-  </si>
-  <si>
     <t>3.A.1</t>
   </si>
   <si>
-    <t>3.A.2</t>
-  </si>
-  <si>
-    <t>3.C.1</t>
-  </si>
-  <si>
     <t>3.C.6</t>
   </si>
   <si>
@@ -4373,15 +4361,9 @@
     <t>3.C.5</t>
   </si>
   <si>
-    <t>3.B.1</t>
-  </si>
-  <si>
     <t>3.B.2</t>
   </si>
   <si>
-    <t>3.B.6</t>
-  </si>
-  <si>
     <t>Agriculture - Rice cultivation (Emissions CH4)</t>
   </si>
   <si>
@@ -4431,6 +4413,42 @@
   </si>
   <si>
     <t>LULUCF - Forest fires</t>
+  </si>
+  <si>
+    <t>3.C.7</t>
+  </si>
+  <si>
+    <t>9.A</t>
+  </si>
+  <si>
+    <t>3.A.2.a</t>
+  </si>
+  <si>
+    <t>3.A.2.b</t>
+  </si>
+  <si>
+    <t>3.A.2.c</t>
+  </si>
+  <si>
+    <t>3.B.1.a</t>
+  </si>
+  <si>
+    <t>3.B.1.b</t>
+  </si>
+  <si>
+    <t>3.B.6.a</t>
+  </si>
+  <si>
+    <t>3.B.6.b</t>
+  </si>
+  <si>
+    <t>3.C.1.a</t>
+  </si>
+  <si>
+    <t>3.C.1.b</t>
+  </si>
+  <si>
+    <t>3.C.1.c</t>
   </si>
 </sst>
 </file>
@@ -7777,15 +7795,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025E69B7-8824-448C-9919-E0CA0E64D7DC}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -7801,7 +7819,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1435</v>
+        <v>1459</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>532</v>
@@ -7812,10 +7830,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1436</v>
+        <v>1458</v>
       </c>
       <c r="B3" t="s">
-        <v>1447</v>
+        <v>1441</v>
       </c>
       <c r="C3" t="s">
         <v>512</v>
@@ -7823,68 +7841,68 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="B4" t="s">
-        <v>1448</v>
+        <v>1444</v>
       </c>
       <c r="C4" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1439</v>
+        <v>1435</v>
       </c>
       <c r="B5" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="C5" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1441</v>
+        <v>1436</v>
       </c>
       <c r="B6" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
       <c r="C6" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1437</v>
+        <v>1460</v>
       </c>
       <c r="B7" t="s">
-        <v>1451</v>
+        <v>1448</v>
       </c>
       <c r="C7" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1438</v>
+        <v>1461</v>
       </c>
       <c r="B8" t="s">
-        <v>1452</v>
+        <v>1449</v>
       </c>
       <c r="C8" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1440</v>
+        <v>1462</v>
       </c>
       <c r="B9" t="s">
-        <v>1453</v>
+        <v>1446</v>
       </c>
       <c r="C9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -7892,51 +7910,51 @@
         <v>1438</v>
       </c>
       <c r="B10" t="s">
-        <v>1454</v>
+        <v>1450</v>
       </c>
       <c r="C10" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="B11" t="s">
-        <v>1455</v>
+        <v>1451</v>
       </c>
       <c r="C11" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B12" t="s">
         <v>1442</v>
       </c>
-      <c r="B12" t="s">
-        <v>1456</v>
-      </c>
       <c r="C12" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B13" t="s">
         <v>1443</v>
       </c>
-      <c r="B13" t="s">
-        <v>1457</v>
-      </c>
       <c r="C13" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1439</v>
+        <v>1469</v>
       </c>
       <c r="B14" t="s">
-        <v>1458</v>
+        <v>1452</v>
       </c>
       <c r="C14" t="s">
         <v>523</v>
@@ -7944,89 +7962,56 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="B15" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="C15" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1445</v>
+        <v>1463</v>
       </c>
       <c r="B16" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="C16" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1444</v>
+        <v>1464</v>
       </c>
       <c r="B17" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="C17" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1444</v>
+        <v>1465</v>
       </c>
       <c r="B18" t="s">
-        <v>1461</v>
+        <v>1456</v>
       </c>
       <c r="C18" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1446</v>
+        <v>1466</v>
       </c>
       <c r="B19" t="s">
-        <v>1462</v>
+        <v>1457</v>
       </c>
       <c r="C19" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>1446</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1462</v>
-      </c>
-      <c r="C20" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>1446</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1463</v>
-      </c>
-      <c r="C21" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>1446</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1463</v>
-      </c>
-      <c r="C22" t="s">
         <v>528</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished dataset and Nigeria example
</commit_message>
<xml_diff>
--- a/gears_db/data/classifications/equivalence.xlsx
+++ b/gears_db/data/classifications/equivalence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\gears\gears_db\data\classifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B58FE36-79C7-45CD-B633-6920754D940B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB89DEDA-F5C4-414B-BBC6-8E1968896CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{1DC89B59-BD96-4A38-B17B-1A23D20B8AC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{1DC89B59-BD96-4A38-B17B-1A23D20B8AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="FAOSTAT COUNTRIES" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2491" uniqueCount="1537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="1538">
   <si>
     <t>Armenia</t>
   </si>
@@ -4651,6 +4651,9 @@
   </si>
   <si>
     <t>Transformation in petrochemical plants</t>
+  </si>
+  <si>
+    <t>9999</t>
   </si>
 </sst>
 </file>
@@ -8901,10 +8904,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63253317-D4D4-44AE-8569-E5504D1816EA}">
-  <dimension ref="A1:B420"/>
+  <dimension ref="A1:B421"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
+      <selection activeCell="A421" sqref="A421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12272,6 +12275,14 @@
         <v>1432</v>
       </c>
     </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A421" s="2" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B421" t="s">
+        <v>1433</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12281,7 +12292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DBF80C-9CB1-41D2-A970-6713DB7EA0BA}">
   <dimension ref="A1:E420"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>